<commit_message>
Sup Info = removed the data table (this will go on Dryad instead of Sup Info). Neg to NEG in the Data2014 table, altered filenames in the figures file.  Added some code to the data checking file.
</commit_message>
<xml_diff>
--- a/VIT_Interval_thru2014.xlsx
+++ b/VIT_Interval_thru2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21840" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VIT_Interval_4" sheetId="1" r:id="rId1"/>
@@ -3372,7 +3372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I558" sqref="I558"/>
     </sheetView>
@@ -28073,8 +28073,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L581"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F563" sqref="F563"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H563" sqref="H563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49481,7 +49481,7 @@
         <v>157</v>
       </c>
       <c r="K563" s="27" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="L563" s="29" t="s">
         <v>157</v>

</xml_diff>